<commit_message>
added 2 methods: check_all_member_sizes and load reference tables
</commit_message>
<xml_diff>
--- a/tables/input/trial1_kotik.xlsx
+++ b/tables/input/trial1_kotik.xlsx
@@ -114,10 +114,10 @@
     <t>L5-S2</t>
   </si>
   <si>
-    <t xml:space="preserve">P (kN/m) </t>
-  </si>
-  <si>
     <t xml:space="preserve"> θ (Deg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ned (kN) </t>
   </si>
 </sst>
 </file>
@@ -165,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -261,27 +261,40 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="8"/>
-      </left>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -289,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -313,12 +326,23 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1482,8 +1506,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:IV38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1538,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1534,22 +1558,22 @@
       <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="P1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="18" t="s">
         <v>16</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -1576,7 +1600,7 @@
         <v>12.5</v>
       </c>
       <c r="F2" s="5">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G2" s="5">
         <v>90</v>
@@ -1599,22 +1623,22 @@
       <c r="M2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="14">
         <v>1</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="23">
         <v>1</v>
       </c>
-      <c r="P2" s="18">
-        <v>686</v>
-      </c>
-      <c r="Q2" s="15">
+      <c r="P2" s="24">
+        <v>4122</v>
+      </c>
+      <c r="Q2" s="23">
         <v>50</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="23">
         <v>355</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T2" s="5">
@@ -1641,7 +1665,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G3" s="5">
         <v>45</v>
@@ -1664,22 +1688,22 @@
       <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="14">
         <v>1</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="23">
         <v>1</v>
       </c>
-      <c r="P3" s="18">
-        <v>686</v>
-      </c>
-      <c r="Q3" s="15">
+      <c r="P3" s="24">
+        <v>4122</v>
+      </c>
+      <c r="Q3" s="23">
         <v>50</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="23">
         <v>355</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T3" s="5">
@@ -1706,7 +1730,7 @@
         <v>12.5</v>
       </c>
       <c r="F4" s="5">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G4" s="5">
         <v>90</v>
@@ -1729,22 +1753,22 @@
       <c r="M4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="14">
         <v>1</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="23">
         <v>1</v>
       </c>
-      <c r="P4" s="18">
-        <v>1164</v>
-      </c>
-      <c r="Q4" s="15">
+      <c r="P4" s="24">
+        <v>6987</v>
+      </c>
+      <c r="Q4" s="23">
         <v>50</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="23">
         <v>355</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T4" s="5">
@@ -1771,7 +1795,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G5" s="5">
         <v>45</v>
@@ -1794,22 +1818,22 @@
       <c r="M5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="14">
         <v>1</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="23">
         <v>1</v>
       </c>
-      <c r="P5" s="18">
-        <v>1164</v>
-      </c>
-      <c r="Q5" s="15">
+      <c r="P5" s="24">
+        <v>6987</v>
+      </c>
+      <c r="Q5" s="23">
         <v>50</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="23">
         <v>355</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T5" s="5">
@@ -1836,7 +1860,7 @@
         <v>12.5</v>
       </c>
       <c r="F6" s="5">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G6" s="5">
         <v>90</v>
@@ -1859,22 +1883,22 @@
       <c r="M6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="14">
         <v>1</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="23">
         <v>1</v>
       </c>
-      <c r="P6" s="18">
-        <v>1962</v>
-      </c>
-      <c r="Q6" s="15">
+      <c r="P6" s="24">
+        <v>11773</v>
+      </c>
+      <c r="Q6" s="23">
         <v>50</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="23">
         <v>355</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T6" s="5">
@@ -1901,7 +1925,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G7" s="5">
         <v>45</v>
@@ -1924,22 +1948,22 @@
       <c r="M7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="14">
         <v>1</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="23">
         <v>1</v>
       </c>
-      <c r="P7" s="18">
-        <v>1962</v>
-      </c>
-      <c r="Q7" s="15">
+      <c r="P7" s="24">
+        <v>11773</v>
+      </c>
+      <c r="Q7" s="23">
         <v>50</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="23">
         <v>355</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T7" s="5">
@@ -1966,7 +1990,7 @@
         <v>12.5</v>
       </c>
       <c r="F8" s="5">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G8" s="5">
         <v>90</v>
@@ -1989,22 +2013,22 @@
       <c r="M8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="14">
         <v>1</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="23">
         <v>1</v>
       </c>
-      <c r="P8" s="18">
-        <v>1724</v>
-      </c>
-      <c r="Q8" s="15">
+      <c r="P8" s="24">
+        <v>10347</v>
+      </c>
+      <c r="Q8" s="23">
         <v>50</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="23">
         <v>355</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T8" s="5">
@@ -2031,7 +2055,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G9" s="5">
         <v>45</v>
@@ -2054,22 +2078,22 @@
       <c r="M9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="14">
         <v>1</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="23">
         <v>1</v>
       </c>
-      <c r="P9" s="18">
-        <v>1724</v>
-      </c>
-      <c r="Q9" s="15">
+      <c r="P9" s="24">
+        <v>10347</v>
+      </c>
+      <c r="Q9" s="23">
         <v>50</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="23">
         <v>355</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T9" s="5">
@@ -2096,7 +2120,7 @@
         <v>12.5</v>
       </c>
       <c r="F10" s="5">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G10" s="5">
         <v>90</v>
@@ -2119,22 +2143,22 @@
       <c r="M10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="14">
         <v>1</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="23">
         <v>1</v>
       </c>
-      <c r="P10" s="18">
-        <v>960</v>
-      </c>
-      <c r="Q10" s="15">
+      <c r="P10" s="24">
+        <v>5765</v>
+      </c>
+      <c r="Q10" s="23">
         <v>50</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="23">
         <v>355</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T10" s="5">
@@ -2161,7 +2185,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G11" s="5">
         <v>45</v>
@@ -2184,22 +2208,22 @@
       <c r="M11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="14">
         <v>1</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="23">
         <v>1</v>
       </c>
-      <c r="P11" s="18">
-        <v>960</v>
-      </c>
-      <c r="Q11" s="15">
+      <c r="P11" s="24">
+        <v>5765</v>
+      </c>
+      <c r="Q11" s="23">
         <v>50</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="23">
         <v>355</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="T11" s="5">
@@ -2223,12 +2247,12 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="4"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="19"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
@@ -2246,12 +2270,12 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="20"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
     </row>
@@ -2270,10 +2294,10 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>

</xml_diff>

<commit_message>
added dead load calculation
</commit_message>
<xml_diff>
--- a/tables/input/trial1_kotik.xlsx
+++ b/tables/input/trial1_kotik.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DDD\NUS_modules_from PC_ not on drive\5112\KOTIK\strut pack\civilR\tables\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DDD\NUS_modules_from PC_ not on drive\5112\KOTIK\strut pack\civilR 2\civilR\tables\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Strut name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>LL(kN/m)</t>
   </si>
   <si>
-    <t>IL (kN/m)</t>
-  </si>
-  <si>
     <t>steel_grade S</t>
   </si>
   <si>
@@ -118,6 +115,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ned (kN) </t>
+  </si>
+  <si>
+    <t>AL (kN/m)</t>
+  </si>
+  <si>
+    <t>ml(kg/m)</t>
   </si>
 </sst>
 </file>
@@ -151,20 +154,20 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -320,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -343,8 +346,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -357,11 +358,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1523,21 +1528,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV38"/>
+  <dimension ref="A1:IW38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" style="1" customWidth="1"/>
-    <col min="2" max="18" width="8.81640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6328125" style="1" customWidth="1"/>
-    <col min="20" max="256" width="8.81640625" style="1" customWidth="1"/>
+    <col min="2" max="13" width="8.81640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" style="28" customWidth="1"/>
+    <col min="15" max="19" width="8.81640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6328125" style="1" customWidth="1"/>
+    <col min="21" max="257" width="8.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1577,34 +1584,37 @@
       <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="S1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="T1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="U1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5">
         <v>12.5</v>
@@ -1640,36 +1650,39 @@
         <v>210</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="24">
+        <v>1</v>
+      </c>
+      <c r="O2" s="19">
+        <v>1</v>
+      </c>
+      <c r="P2" s="19">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>4122</v>
+      </c>
+      <c r="R2" s="19">
+        <v>50</v>
+      </c>
+      <c r="S2" s="19">
+        <v>355</v>
+      </c>
+      <c r="T2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="25">
-        <v>1</v>
-      </c>
-      <c r="O2" s="21">
-        <v>1</v>
-      </c>
-      <c r="P2" s="26">
-        <v>4122</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>50</v>
-      </c>
-      <c r="R2" s="21">
-        <v>355</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="5">
+      <c r="U2" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U2" s="5">
+      <c r="V2" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5">
         <v>7</v>
@@ -1705,36 +1718,39 @@
         <v>210</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="24">
+        <v>1</v>
+      </c>
+      <c r="O3" s="19">
+        <v>1</v>
+      </c>
+      <c r="P3" s="19">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>4122</v>
+      </c>
+      <c r="R3" s="19">
+        <v>50</v>
+      </c>
+      <c r="S3" s="19">
+        <v>355</v>
+      </c>
+      <c r="T3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="25">
-        <v>1</v>
-      </c>
-      <c r="O3" s="21">
-        <v>1</v>
-      </c>
-      <c r="P3" s="26">
-        <v>4122</v>
-      </c>
-      <c r="Q3" s="21">
-        <v>50</v>
-      </c>
-      <c r="R3" s="21">
-        <v>355</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="5">
+      <c r="U3" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U3" s="5">
+      <c r="V3" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5">
         <v>12.5</v>
@@ -1772,34 +1788,37 @@
       <c r="M4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="24">
         <v>1</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="19">
         <v>1</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="19">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="Q4" s="20">
         <v>6987</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="R4" s="19">
         <v>50</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="19">
         <v>355</v>
       </c>
-      <c r="S4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T4" s="5">
+      <c r="T4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U4" s="5">
+      <c r="V4" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5">
         <v>7</v>
@@ -1837,34 +1856,37 @@
       <c r="M5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="19">
         <v>1</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="19">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="Q5" s="20">
         <v>6987</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="R5" s="19">
         <v>50</v>
       </c>
-      <c r="R5" s="21">
+      <c r="S5" s="19">
         <v>355</v>
       </c>
-      <c r="S5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5" s="5">
+      <c r="T5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U5" s="5">
+      <c r="V5" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5">
         <v>12.5</v>
@@ -1894,7 +1916,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L6" s="5">
         <v>210</v>
@@ -1902,34 +1924,37 @@
       <c r="M6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="24">
         <v>1</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="19">
         <v>1</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q6" s="20">
         <v>11773</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="R6" s="19">
         <v>50</v>
       </c>
-      <c r="R6" s="21">
+      <c r="S6" s="19">
         <v>355</v>
       </c>
-      <c r="S6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T6" s="5">
+      <c r="T6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U6" s="5">
+      <c r="V6" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>7</v>
@@ -1959,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L7" s="5">
         <v>210</v>
@@ -1967,34 +1992,37 @@
       <c r="M7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="24">
         <v>1</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="19">
         <v>1</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q7" s="20">
         <v>11773</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="R7" s="19">
         <v>50</v>
       </c>
-      <c r="R7" s="21">
+      <c r="S7" s="19">
         <v>355</v>
       </c>
-      <c r="S7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T7" s="5">
+      <c r="T7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U7" s="5">
+      <c r="V7" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <v>12.5</v>
@@ -2024,7 +2052,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L8" s="5">
         <v>210</v>
@@ -2032,34 +2060,37 @@
       <c r="M8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="24">
         <v>1</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="19">
         <v>1</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q8" s="20">
         <v>10347</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="R8" s="19">
         <v>50</v>
       </c>
-      <c r="R8" s="21">
+      <c r="S8" s="19">
         <v>355</v>
       </c>
-      <c r="S8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="5">
+      <c r="T8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U8" s="5">
+      <c r="V8" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5">
         <v>7</v>
@@ -2089,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L9" s="5">
         <v>210</v>
@@ -2097,34 +2128,37 @@
       <c r="M9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="24">
         <v>1</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="19">
         <v>1</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q9" s="20">
         <v>10347</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="R9" s="19">
         <v>50</v>
       </c>
-      <c r="R9" s="21">
+      <c r="S9" s="19">
         <v>355</v>
       </c>
-      <c r="S9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T9" s="5">
+      <c r="T9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U9" s="5">
+      <c r="V9" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5">
         <v>12.5</v>
@@ -2154,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L10" s="5">
         <v>210</v>
@@ -2162,34 +2196,37 @@
       <c r="M10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="24">
         <v>1</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="19">
         <v>1</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q10" s="20">
         <v>5765</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="R10" s="19">
         <v>50</v>
       </c>
-      <c r="R10" s="21">
+      <c r="S10" s="19">
         <v>355</v>
       </c>
-      <c r="S10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T10" s="5">
+      <c r="T10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U10" s="5">
+      <c r="V10" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5">
         <v>7</v>
@@ -2219,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="5">
-        <v>1510</v>
+        <v>2270</v>
       </c>
       <c r="L11" s="5">
         <v>210</v>
@@ -2227,32 +2264,35 @@
       <c r="M11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="24">
         <v>1</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="19">
         <v>1</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="19">
+        <v>17.8</v>
+      </c>
+      <c r="Q11" s="20">
         <v>5765</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="R11" s="19">
         <v>50</v>
       </c>
-      <c r="R11" s="21">
+      <c r="S11" s="19">
         <v>355</v>
       </c>
-      <c r="S11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T11" s="5">
+      <c r="T11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="U11" s="5">
+      <c r="V11" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2266,16 +2306,17 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="7"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="15"/>
       <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2289,16 +2330,17 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="8"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="16"/>
       <c r="U13" s="8"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V13" s="8"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -2312,16 +2354,17 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="9"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -2335,7 +2378,7 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="N15" s="27"/>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
@@ -2343,8 +2386,9 @@
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V15" s="9"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -2358,7 +2402,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="N16" s="27"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
@@ -2366,8 +2410,9 @@
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V16" s="9"/>
+    </row>
+    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2381,7 +2426,7 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="N17" s="27"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -2389,8 +2434,9 @@
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -2404,7 +2450,7 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
+      <c r="N18" s="27"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
@@ -2412,8 +2458,9 @@
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
-    </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2427,7 +2474,7 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
@@ -2435,8 +2482,9 @@
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2450,7 +2498,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="N20" s="27"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -2458,8 +2506,9 @@
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
-    </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V20" s="9"/>
+    </row>
+    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -2473,7 +2522,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
+      <c r="N21" s="27"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
@@ -2481,8 +2530,9 @@
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V21" s="9"/>
+    </row>
+    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2496,7 +2546,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
+      <c r="N22" s="27"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
@@ -2504,8 +2554,9 @@
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
-    </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V22" s="9"/>
+    </row>
+    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2519,7 +2570,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
@@ -2527,8 +2578,9 @@
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
-    </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V23" s="9"/>
+    </row>
+    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2542,7 +2594,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
+      <c r="N24" s="27"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
@@ -2550,8 +2602,9 @@
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
-    </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V24" s="9"/>
+    </row>
+    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2565,7 +2618,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="11"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
+      <c r="N25" s="27"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
@@ -2573,8 +2626,9 @@
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
       <c r="U25" s="9"/>
-    </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V25" s="9"/>
+    </row>
+    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2588,7 +2642,7 @@
       <c r="K26" s="11"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
@@ -2596,8 +2650,9 @@
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
       <c r="U26" s="9"/>
-    </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V26" s="9"/>
+    </row>
+    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -2611,7 +2666,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
@@ -2619,8 +2674,9 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
-    </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V27" s="9"/>
+    </row>
+    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -2634,7 +2690,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
+      <c r="N28" s="27"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
@@ -2642,8 +2698,9 @@
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
       <c r="U28" s="9"/>
-    </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V28" s="9"/>
+    </row>
+    <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2657,7 +2714,7 @@
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
@@ -2665,8 +2722,9 @@
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
       <c r="U29" s="9"/>
-    </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V29" s="9"/>
+    </row>
+    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2680,7 +2738,7 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
+      <c r="N30" s="27"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
@@ -2688,8 +2746,9 @@
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
       <c r="U30" s="9"/>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -2703,7 +2762,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
+      <c r="N31" s="27"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
@@ -2711,8 +2770,9 @@
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
-    </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -2726,7 +2786,7 @@
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
+      <c r="N32" s="27"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
@@ -2734,8 +2794,9 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
       <c r="U32" s="9"/>
-    </row>
-    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -2749,7 +2810,7 @@
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
+      <c r="N33" s="27"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
@@ -2757,8 +2818,9 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
-    </row>
-    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2772,7 +2834,7 @@
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="N34" s="27"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
@@ -2780,8 +2842,9 @@
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
       <c r="U34" s="9"/>
-    </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V34" s="9"/>
+    </row>
+    <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -2795,7 +2858,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
+      <c r="N35" s="27"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
@@ -2803,8 +2866,9 @@
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V35" s="9"/>
+    </row>
+    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -2818,7 +2882,7 @@
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
+      <c r="N36" s="27"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
@@ -2826,8 +2890,9 @@
       <c r="S36" s="9"/>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
-    </row>
-    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V36" s="9"/>
+    </row>
+    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2841,7 +2906,7 @@
       <c r="K37" s="11"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
+      <c r="N37" s="27"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
@@ -2849,8 +2914,9 @@
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
-    </row>
-    <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V37" s="9"/>
+    </row>
+    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2864,7 +2930,7 @@
       <c r="K38" s="11"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="N38" s="27"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
@@ -2872,6 +2938,7 @@
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>